<commit_message>
Update to complete DCPU with hazard.
Signed-off-by: David Qiu <david@davidqiu.com>
</commit_message>
<xml_diff>
--- a/Documents/D-CPU Design Specifications/D-CPU Design Specifications.xlsx
+++ b/Documents/D-CPU Design Specifications/D-CPU Design Specifications.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="600" yWindow="120" windowWidth="19395" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Operations" sheetId="1" r:id="rId1"/>
+    <sheet name="CPU Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="ALU Operations" sheetId="3" r:id="rId2"/>
     <sheet name="Registers" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -18,10 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="302">
   <si>
-    <t>Operation List</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mnemonic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2488,6 +2484,10 @@
   </si>
   <si>
     <t>ALU_SRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Central Processer Unit Instruction List</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2734,9 +2734,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2747,6 +2744,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3052,8 +3052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -3073,1311 +3073,1311 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="A1" s="35" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="D2" s="33" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="D2" s="32" t="s">
         <v>270</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="F2" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:13" ht="33" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="I3" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="34">
-        <v>0</v>
-      </c>
-      <c r="J4" s="34">
-        <v>0</v>
-      </c>
-      <c r="K4" s="34">
-        <v>0</v>
-      </c>
-      <c r="L4" s="34">
-        <v>0</v>
-      </c>
-      <c r="M4" s="34" t="s">
-        <v>288</v>
+        <v>53</v>
+      </c>
+      <c r="I4" s="33">
+        <v>0</v>
+      </c>
+      <c r="J4" s="33">
+        <v>0</v>
+      </c>
+      <c r="K4" s="33">
+        <v>0</v>
+      </c>
+      <c r="L4" s="33">
+        <v>0</v>
+      </c>
+      <c r="M4" s="33" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>154</v>
-      </c>
       <c r="G5" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="34">
-        <v>0</v>
-      </c>
-      <c r="J5" s="34">
-        <v>0</v>
-      </c>
-      <c r="K5" s="34">
-        <v>0</v>
-      </c>
-      <c r="L5" s="34">
-        <v>0</v>
-      </c>
-      <c r="M5" s="34" t="s">
-        <v>288</v>
+        <v>20</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>0</v>
+      </c>
+      <c r="K5" s="33">
+        <v>0</v>
+      </c>
+      <c r="L5" s="33">
+        <v>0</v>
+      </c>
+      <c r="M5" s="33" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="D6" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="J6" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="K6" s="34">
+      <c r="K6" s="33">
         <v>0</v>
       </c>
       <c r="L6" s="14">
         <v>0</v>
       </c>
-      <c r="M6" s="35" t="s">
-        <v>289</v>
+      <c r="M6" s="34" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="34">
-        <v>0</v>
-      </c>
-      <c r="J7" s="34">
+        <v>50</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
         <v>0</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="L7" s="34">
-        <v>0</v>
-      </c>
-      <c r="M7" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
+      </c>
+      <c r="L7" s="33">
+        <v>0</v>
+      </c>
+      <c r="M7" s="33" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B8" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="H8" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="I8" s="34">
+      <c r="I8" s="33">
         <v>0</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K8" s="34">
-        <v>0</v>
-      </c>
-      <c r="L8" s="34">
+        <v>274</v>
+      </c>
+      <c r="K8" s="33">
+        <v>0</v>
+      </c>
+      <c r="L8" s="33">
         <v>0</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I9" s="34">
-        <v>0</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="K9" s="34">
-        <v>0</v>
-      </c>
-      <c r="L9" s="34">
+      <c r="K9" s="33">
+        <v>0</v>
+      </c>
+      <c r="L9" s="33">
         <v>0</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="34">
+      <c r="I10" s="33">
         <v>0</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K10" s="34">
-        <v>0</v>
-      </c>
-      <c r="L10" s="34">
+        <v>274</v>
+      </c>
+      <c r="K10" s="33">
+        <v>0</v>
+      </c>
+      <c r="L10" s="33">
         <v>0</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="I11" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K11" s="34">
+        <v>274</v>
+      </c>
+      <c r="K11" s="33">
         <v>0</v>
       </c>
       <c r="L11" s="14">
         <v>0</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K12" s="34">
+        <v>274</v>
+      </c>
+      <c r="K12" s="33">
         <v>0</v>
       </c>
       <c r="L12" s="14">
         <v>0</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="I13" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K13" s="34">
+        <v>274</v>
+      </c>
+      <c r="K13" s="33">
         <v>0</v>
       </c>
       <c r="L13" s="14">
         <v>0</v>
       </c>
       <c r="M13" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K14" s="34">
+        <v>274</v>
+      </c>
+      <c r="K14" s="33">
         <v>0</v>
       </c>
       <c r="L14" s="14">
         <v>0</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K15" s="34">
+        <v>274</v>
+      </c>
+      <c r="K15" s="33">
         <v>0</v>
       </c>
       <c r="L15" s="14">
         <v>0</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="I16" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K16" s="34">
+        <v>274</v>
+      </c>
+      <c r="K16" s="33">
         <v>0</v>
       </c>
       <c r="L16" s="14">
         <v>0</v>
       </c>
       <c r="M16" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="H17" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K17" s="34">
+        <v>274</v>
+      </c>
+      <c r="K17" s="33">
         <v>0</v>
       </c>
       <c r="L17" s="14">
         <v>0</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B18" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K18" s="34">
+        <v>274</v>
+      </c>
+      <c r="K18" s="33">
         <v>0</v>
       </c>
       <c r="L18" s="14">
         <v>0</v>
       </c>
       <c r="M18" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>247</v>
-      </c>
       <c r="G19" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K19" s="34">
+        <v>274</v>
+      </c>
+      <c r="K19" s="33">
         <v>0</v>
       </c>
       <c r="L19" s="14">
         <v>0</v>
       </c>
       <c r="M19" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="F20" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K20" s="34">
+        <v>284</v>
+      </c>
+      <c r="K20" s="33">
         <v>0</v>
       </c>
       <c r="L20" s="14">
         <v>0</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K21" s="34">
+        <v>274</v>
+      </c>
+      <c r="K21" s="33">
         <v>0</v>
       </c>
       <c r="L21" s="14">
         <v>0</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="F22" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K22" s="34">
+        <v>284</v>
+      </c>
+      <c r="K22" s="33">
         <v>0</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M22" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="I23" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K23" s="34">
+        <v>284</v>
+      </c>
+      <c r="K23" s="33">
         <v>0</v>
       </c>
       <c r="L23" s="14">
         <v>0</v>
       </c>
       <c r="M23" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="I24" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K24" s="34">
+        <v>274</v>
+      </c>
+      <c r="K24" s="33">
         <v>0</v>
       </c>
       <c r="L24" s="14">
         <v>0</v>
       </c>
       <c r="M24" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>231</v>
-      </c>
       <c r="H25" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="K25" s="33">
+        <v>0</v>
+      </c>
+      <c r="L25" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="I25" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="K25" s="34">
-        <v>0</v>
-      </c>
-      <c r="L25" s="14" t="s">
-        <v>280</v>
-      </c>
       <c r="M25" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B26" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="F26" s="23" t="s">
-        <v>185</v>
-      </c>
       <c r="G26" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H26" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="H26" s="15" t="s">
-        <v>196</v>
-      </c>
       <c r="I26" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="J26" s="34">
-        <v>0</v>
-      </c>
-      <c r="K26" s="34">
-        <v>0</v>
-      </c>
-      <c r="L26" s="34">
+        <v>280</v>
+      </c>
+      <c r="J26" s="33">
+        <v>0</v>
+      </c>
+      <c r="K26" s="33">
+        <v>0</v>
+      </c>
+      <c r="L26" s="33">
         <v>0</v>
       </c>
       <c r="M26" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B27" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K27" s="34">
-        <v>0</v>
-      </c>
-      <c r="L27" s="34">
+        <v>284</v>
+      </c>
+      <c r="K27" s="33">
+        <v>0</v>
+      </c>
+      <c r="L27" s="33">
         <v>0</v>
       </c>
       <c r="M27" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B28" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="C28" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="H28" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="H28" s="15" t="s">
-        <v>260</v>
-      </c>
       <c r="I28" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="K28" s="34">
+        <v>274</v>
+      </c>
+      <c r="K28" s="33">
         <v>0</v>
       </c>
       <c r="L28" s="14">
         <v>0</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="H29" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="I29" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K29" s="34">
-        <v>0</v>
-      </c>
-      <c r="L29" s="34">
+        <v>284</v>
+      </c>
+      <c r="K29" s="33">
+        <v>0</v>
+      </c>
+      <c r="L29" s="33">
         <v>0</v>
       </c>
       <c r="M29" s="14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="F30" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K30" s="34">
-        <v>0</v>
-      </c>
-      <c r="L30" s="34">
+        <v>284</v>
+      </c>
+      <c r="K30" s="33">
+        <v>0</v>
+      </c>
+      <c r="L30" s="33">
         <v>0</v>
       </c>
       <c r="M30" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B31" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="G31" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H31" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="I31" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K31" s="34">
-        <v>0</v>
-      </c>
-      <c r="L31" s="34">
+        <v>284</v>
+      </c>
+      <c r="K31" s="33">
+        <v>0</v>
+      </c>
+      <c r="L31" s="33">
         <v>0</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="G32" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J32" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K32" s="34">
-        <v>0</v>
-      </c>
-      <c r="L32" s="34">
+        <v>284</v>
+      </c>
+      <c r="K32" s="33">
+        <v>0</v>
+      </c>
+      <c r="L32" s="33">
         <v>0</v>
       </c>
       <c r="M32" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="G33" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K33" s="34">
-        <v>0</v>
-      </c>
-      <c r="L33" s="34">
+        <v>284</v>
+      </c>
+      <c r="K33" s="33">
+        <v>0</v>
+      </c>
+      <c r="L33" s="33">
         <v>0</v>
       </c>
       <c r="M33" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="F34" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K34" s="34">
-        <v>0</v>
-      </c>
-      <c r="L34" s="34">
+        <v>284</v>
+      </c>
+      <c r="K34" s="33">
+        <v>0</v>
+      </c>
+      <c r="L34" s="33">
         <v>0</v>
       </c>
       <c r="M34" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="F35" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K35" s="34">
-        <v>0</v>
-      </c>
-      <c r="L35" s="34">
+        <v>284</v>
+      </c>
+      <c r="K35" s="33">
+        <v>0</v>
+      </c>
+      <c r="L35" s="33">
         <v>0</v>
       </c>
       <c r="M35" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.3">
@@ -4425,522 +4425,522 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="A1" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="I3" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="I3" s="28" t="s">
-        <v>214</v>
-      </c>
       <c r="J3" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4" s="5">
         <v>0</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>227</v>
-      </c>
       <c r="J5" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F6" s="5">
         <v>0</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F7" s="5">
         <v>0</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="J9" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F10" s="21">
         <v>0</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="E12" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>174</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>174</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>174</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>174</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -4971,25 +4971,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="A1" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -4997,13 +4997,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -5016,13 +5016,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -5035,10 +5035,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="25"/>
     </row>
@@ -5052,13 +5052,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -5066,13 +5066,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -5080,10 +5080,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11" s="25"/>
     </row>
@@ -5092,10 +5092,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D12" s="25"/>
     </row>
@@ -5104,10 +5104,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" s="25"/>
     </row>
@@ -5116,13 +5116,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update specification, data hazard finished, instruction LOAD lacks of test.
Signed-off-by: David Qiu <david@davidqiu.com>
</commit_message>
<xml_diff>
--- a/Documents/D-CPU Design Specifications/D-CPU Design Specifications.xlsx
+++ b/Documents/D-CPU Design Specifications/D-CPU Design Specifications.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="305">
   <si>
     <t>Mnemonic</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -399,10 +399,6 @@
       </rPr>
       <t>MMEDIATE</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Control</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2262,232 +2258,248 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>r1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">RANCH </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑 Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>QUAL</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if ZF=1 branch to r1+{val2, val3}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if ZF=0 &amp; NF=0 branch to r1+{val2, val3}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if ZF=0 &amp; NF=1 branch to r1+{val2, val3}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if NF=0 branch to r1+{val2, val3}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXRB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXSD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXCF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inst[3:0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inst[7:4]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inst[10:8]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inst[15:11]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAL3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{VAL2,VAL3}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r1 &lt;- {val2, val3, 0000_0000} (lower 8’b0 can be given with ADDI)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{VAL2,VAL3,8'b0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OCF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r1 &lt;- r2-r3-CF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OCF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input2 -&gt; Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_LOAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_ADDC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_ADDC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_SUBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_INC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_CMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_ADDC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_XOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_AND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_OR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_SLL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_SLA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_SRL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU_SRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Central Processer Unit Instruction List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>BE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>r1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>val3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">RANCH </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑 Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>QUAL</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if ZF=1 branch to r1+{val2, val3}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if ZF=0 &amp; NF=0 branch to r1+{val2, val3}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if ZF=0 &amp; NF=1 branch to r1+{val2, val3}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if NF=0 branch to r1+{val2, val3}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXRB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXSD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXCF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXRA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CALL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inst[3:0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inst[7:4]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inst[10:8]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inst[15:11]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VAL3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{VAL2,VAL3}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r1 &lt;- {val2, val3, 0000_0000} (lower 8’b0 can be given with ADDI)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{VAL2,VAL3,8'b0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OCF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r1 &lt;- r2-r3-CF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OCF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input2 -&gt; Output</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_LOAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_ADDC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_ADDC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_SUBB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_INC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_CMP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_ADDC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_XOR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_AND</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_OR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_SLL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_SLA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_SRL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALU_SRA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Central Processer Unit Instruction List</t>
+    <t>&lt;ANY&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ANY&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ANY&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ANY&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2640,7 +2652,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2747,6 +2759,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3052,8 +3067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -3074,7 +3089,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="35" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -3088,16 +3103,16 @@
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="32" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
@@ -3113,13 +3128,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="F3" s="26" t="s">
         <v>203</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>204</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>54</v>
@@ -3128,19 +3143,19 @@
         <v>2</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J3" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -3154,13 +3169,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>56</v>
@@ -3168,11 +3183,11 @@
       <c r="H4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="33">
-        <v>0</v>
-      </c>
-      <c r="J4" s="33">
-        <v>0</v>
+      <c r="I4" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>302</v>
       </c>
       <c r="K4" s="33">
         <v>0</v>
@@ -3181,24 +3196,24 @@
         <v>0</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E5" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>152</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>153</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>55</v>
@@ -3206,11 +3221,11 @@
       <c r="H5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="33">
-        <v>0</v>
-      </c>
-      <c r="J5" s="33">
-        <v>0</v>
+      <c r="I5" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>302</v>
       </c>
       <c r="K5" s="33">
         <v>0</v>
@@ -3219,21 +3234,21 @@
         <v>0</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>6</v>
@@ -3248,10 +3263,10 @@
         <v>49</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K6" s="33">
         <v>0</v>
@@ -3260,11 +3275,11 @@
         <v>0</v>
       </c>
       <c r="M6" s="34" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -3285,110 +3300,113 @@
       <c r="H7" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="33">
-        <v>0</v>
-      </c>
-      <c r="J7" s="33">
-        <v>0</v>
+      <c r="I7" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>271</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="L7" s="33">
-        <v>0</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" s="15" t="s">
+      <c r="D8" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="K8" s="33">
+        <v>0</v>
+      </c>
+      <c r="L8" s="33">
+        <v>0</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="I8" s="33">
-        <v>0</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="K8" s="33">
-        <v>0</v>
-      </c>
-      <c r="L8" s="33">
-        <v>0</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="K9" s="33">
+        <v>0</v>
+      </c>
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="I9" s="33">
-        <v>0</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="K9" s="33">
-        <v>0</v>
-      </c>
-      <c r="L9" s="33">
-        <v>0</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>144</v>
-      </c>
       <c r="D10" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>9</v>
@@ -3397,16 +3415,16 @@
         <v>7</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="33">
-        <v>0</v>
+      <c r="I10" s="33" t="s">
+        <v>304</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K10" s="33">
         <v>0</v>
@@ -3415,15 +3433,15 @@
         <v>0</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="30" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>5</v>
@@ -3435,16 +3453,16 @@
         <v>7</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K11" s="33">
         <v>0</v>
@@ -3453,15 +3471,15 @@
         <v>0</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="30" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
@@ -3473,16 +3491,16 @@
         <v>7</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>34</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K12" s="33">
         <v>0</v>
@@ -3491,15 +3509,15 @@
         <v>0</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="30" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
@@ -3511,16 +3529,16 @@
         <v>7</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K13" s="33">
         <v>0</v>
@@ -3529,15 +3547,15 @@
         <v>0</v>
       </c>
       <c r="M13" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
@@ -3549,16 +3567,16 @@
         <v>7</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>37</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K14" s="33">
         <v>0</v>
@@ -3567,53 +3585,53 @@
         <v>0</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="30" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="K15" s="33">
+        <v>0</v>
+      </c>
+      <c r="L15" s="14">
+        <v>0</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="K15" s="33">
-        <v>0</v>
-      </c>
-      <c r="L15" s="14">
-        <v>0</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
@@ -3625,16 +3643,16 @@
         <v>7</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K16" s="33">
         <v>0</v>
@@ -3643,36 +3661,36 @@
         <v>0</v>
       </c>
       <c r="M16" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="30" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="H17" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K17" s="33">
         <v>0</v>
@@ -3681,74 +3699,74 @@
         <v>0</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="K18" s="33">
+        <v>0</v>
+      </c>
+      <c r="L18" s="14">
+        <v>0</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B19" s="36" t="s">
         <v>242</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C19" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="F19" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="H18" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="K18" s="33">
-        <v>0</v>
-      </c>
-      <c r="L18" s="14">
-        <v>0</v>
-      </c>
-      <c r="M18" s="14" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B19" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>250</v>
-      </c>
       <c r="H19" s="15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K19" s="33">
         <v>0</v>
@@ -3757,18 +3775,18 @@
         <v>0</v>
       </c>
       <c r="M19" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>5</v>
@@ -3786,10 +3804,10 @@
         <v>51</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K20" s="33">
         <v>0</v>
@@ -3798,15 +3816,15 @@
         <v>0</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="30" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
@@ -3824,10 +3842,10 @@
         <v>52</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K21" s="33">
         <v>0</v>
@@ -3836,15 +3854,15 @@
         <v>0</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>5</v>
@@ -3856,92 +3874,92 @@
         <v>10</v>
       </c>
       <c r="G22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="K22" s="33">
+        <v>0</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="M22" s="14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="K22" s="33">
-        <v>0</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="M22" s="14" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="10" t="s">
+      <c r="H23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="K23" s="33">
+        <v>0</v>
+      </c>
+      <c r="L23" s="14">
+        <v>0</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="D24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="K23" s="33">
-        <v>0</v>
-      </c>
-      <c r="L23" s="14">
-        <v>0</v>
-      </c>
-      <c r="M23" s="14" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" s="5" t="s">
+      <c r="H24" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="I24" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K24" s="33">
         <v>0</v>
@@ -3950,74 +3968,74 @@
         <v>0</v>
       </c>
       <c r="M24" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>230</v>
-      </c>
       <c r="H25" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="I25" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="I25" s="14" t="s">
-        <v>280</v>
-      </c>
       <c r="J25" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K25" s="33">
         <v>0</v>
       </c>
       <c r="L25" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="M25" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="F26" s="23" t="s">
-        <v>184</v>
-      </c>
       <c r="G26" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="H26" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H26" s="15" t="s">
-        <v>195</v>
-      </c>
       <c r="I26" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="J26" s="33">
-        <v>0</v>
+        <v>278</v>
+      </c>
+      <c r="J26" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="K26" s="33">
         <v>0</v>
@@ -4026,36 +4044,39 @@
         <v>0</v>
       </c>
       <c r="M26" s="14" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="13" t="s">
-        <v>22</v>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>138</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>280</v>
+        <v>239</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>301</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="K27" s="33">
         <v>0</v>
@@ -4064,36 +4085,33 @@
         <v>0</v>
       </c>
       <c r="M27" s="14" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A28" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>255</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="30" t="s">
+        <v>19</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>282</v>
+        <v>252</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>301</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>274</v>
@@ -4101,60 +4119,60 @@
       <c r="K28" s="33">
         <v>0</v>
       </c>
-      <c r="L28" s="14">
+      <c r="L28" s="33">
         <v>0</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B29" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="30" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="K29" s="33">
+        <v>0</v>
+      </c>
+      <c r="L29" s="33">
+        <v>0</v>
+      </c>
+      <c r="M29" s="14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="K29" s="33">
-        <v>0</v>
-      </c>
-      <c r="L29" s="33">
-        <v>0</v>
-      </c>
-      <c r="M29" s="14" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>5</v>
@@ -4166,54 +4184,54 @@
         <v>10</v>
       </c>
       <c r="G30" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="K30" s="33">
+        <v>0</v>
+      </c>
+      <c r="L30" s="33">
+        <v>0</v>
+      </c>
+      <c r="M30" s="14" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="H30" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="K30" s="33">
-        <v>0</v>
-      </c>
-      <c r="L30" s="33">
-        <v>0</v>
-      </c>
-      <c r="M30" s="14" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G31" s="9" t="s">
+      <c r="H31" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H31" s="8" t="s">
-        <v>91</v>
-      </c>
       <c r="I31" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K31" s="33">
         <v>0</v>
@@ -4222,18 +4240,18 @@
         <v>0</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B32" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="30" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
@@ -4245,16 +4263,16 @@
         <v>7</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J32" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K32" s="33">
         <v>0</v>
@@ -4263,15 +4281,15 @@
         <v>0</v>
       </c>
       <c r="M32" s="14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="30" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>5</v>
@@ -4283,16 +4301,16 @@
         <v>7</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K33" s="33">
         <v>0</v>
@@ -4301,7 +4319,7 @@
         <v>0</v>
       </c>
       <c r="M33" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
@@ -4309,28 +4327,28 @@
         <v>27</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="F34" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K34" s="33">
         <v>0</v>
@@ -4339,7 +4357,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
@@ -4347,28 +4365,28 @@
         <v>29</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="F35" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K35" s="33">
         <v>0</v>
@@ -4377,7 +4395,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.3">
@@ -4426,7 +4444,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -4446,19 +4464,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>1</v>
@@ -4471,476 +4489,476 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>201</v>
+      <c r="A3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="21">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="H3" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="I3" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>234</v>
-      </c>
       <c r="I4" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>226</v>
-      </c>
       <c r="J5" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F6" s="5">
         <v>0</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F7" s="5">
         <v>0</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="J9" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="23" t="s">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="F10" s="21">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>251</v>
+      <c r="F10" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>66</v>
+        <v>240</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>212</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>174</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>172</v>
-      </c>
       <c r="E12" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>173</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>173</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>173</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>173</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4972,7 +4990,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -4980,16 +4998,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -4997,13 +5015,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -5016,13 +5034,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -5035,10 +5053,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" s="25"/>
     </row>
@@ -5052,13 +5070,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -5066,13 +5084,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -5080,10 +5098,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" s="25"/>
     </row>
@@ -5092,10 +5110,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12" s="25"/>
     </row>
@@ -5104,10 +5122,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" s="25"/>
     </row>
@@ -5116,13 +5134,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>